<commit_message>
Add support for ExcelIgnoreAttribute and throw for recursive structures
</commit_message>
<xml_diff>
--- a/tests/Resources/Primitives.xlsx
+++ b/tests/Resources/Primitives.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugh/Documents/GitHub/excel-mapper/tests/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE6DD17-6A6F-D142-B27C-CF0196379D34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F68BF11-CE0B-ED40-A2F4-55D329DA3B9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Int Value</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>s4</t>
+  </si>
+  <si>
+    <t>IntValue</t>
   </si>
 </sst>
 </file>
@@ -1598,10 +1601,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B1000"/>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1611,41 +1614,56 @@
     <col min="3" max="27" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>28</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>